<commit_message>
Measure of processing and an error while saving file was added.
- Fixed error for xls format: when file was been saving in xlsx after a xls process it generated an error because extension file didn't change.
- Added Timer for measuring time or processing for every format.
- Added a window to see time elapsed for process.
</commit_message>
<xml_diff>
--- a/AsposeDemo/bin/Debug/templates/report.xlsx
+++ b/AsposeDemo/bin/Debug/templates/report.xlsx
@@ -51,7 +51,7 @@
     <t xml:space="preserve"> ANESTHESIA CONTROLLED SUBSTANCE SHEET FOR KIT#  </t>
   </si>
   <si>
-    <t>KIT WAS USED FROM DATE 05 / 01 / 2018   TO DATE 05 / 17 / 2018</t>
+    <t>KIT WAS USED FROM DATE 05 / 01 / 2018   TO DATE 05 / 18 / 2018</t>
   </si>
   <si>
     <t>Demerol 25MG/ML</t>
@@ -1756,7 +1756,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2190750</xdr:colOff>
+      <xdr:colOff>2095500</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>361950</xdr:rowOff>
     </xdr:to>
@@ -1776,7 +1776,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1466850"/>
-          <a:ext cx="2495550" cy="361950"/>
+          <a:ext cx="2400300" cy="361950"/>
         </a:xfrm>
         <a:prstGeom prst="rect"/>
       </xdr:spPr>

</xml_diff>